<commit_message>
Updated sprint backlog for team\n\n- Updated backlog and burndown chart
</commit_message>
<xml_diff>
--- a/sprints/sprint2/Sprint 2 Backlog & Burndown Chart.xlsx
+++ b/sprints/sprint2/Sprint 2 Backlog & Burndown Chart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Desktop\CS Courses\CS3212\SE2 Project\UWG-SE2-Spring22-Team4\sprints\sprint2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{88155928-B92A-4EF2-A25D-2B65B50E9549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{480D480E-53E3-4E79-853F-CFFFC7C4289D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-10910" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -235,6 +235,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -244,7 +245,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -362,13 +362,13 @@
                   <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1415,8 +1415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
+      <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1428,30 +1428,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="8" t="s">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="7"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="8"/>
       <c r="E2" s="5" t="s">
         <v>3</v>
       </c>
@@ -1492,13 +1492,21 @@
       <c r="D4" s="1">
         <v>10</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
+      <c r="E4" s="2">
+        <v>10</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="9"/>
+      <c r="A5" s="6"/>
       <c r="B5" s="1" t="s">
         <v>32</v>
       </c>
@@ -1508,13 +1516,21 @@
       <c r="D5" s="1">
         <v>10</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
+      <c r="E5" s="2">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="9"/>
+      <c r="A6" s="6"/>
       <c r="B6" s="1" t="s">
         <v>31</v>
       </c>
@@ -1524,10 +1540,18 @@
       <c r="D6" s="1">
         <v>5</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
+      <c r="E6" s="2">
+        <v>5</v>
+      </c>
+      <c r="F6" s="2">
+        <v>5</v>
+      </c>
+      <c r="G6" s="2">
+        <v>5</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
@@ -1540,10 +1564,18 @@
       <c r="D7" s="1">
         <v>10</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+      <c r="E7" s="2">
+        <v>5</v>
+      </c>
+      <c r="F7" s="2">
+        <v>5</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
@@ -1556,10 +1588,18 @@
       <c r="D8" s="1">
         <v>10</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
+      <c r="E8" s="2">
+        <v>5</v>
+      </c>
+      <c r="F8" s="2">
+        <v>5</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
@@ -1572,10 +1612,18 @@
       <c r="D9" s="1">
         <v>10</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
+      <c r="E9" s="2">
+        <v>3</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
@@ -1588,10 +1636,18 @@
       <c r="D10" s="1">
         <v>5</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
+      <c r="E10" s="2">
+        <v>8</v>
+      </c>
+      <c r="F10" s="2">
+        <v>8</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
@@ -1606,10 +1662,18 @@
       <c r="D11" s="1">
         <v>1</v>
       </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
+      <c r="E11" s="2">
+        <v>1</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
@@ -1622,10 +1686,18 @@
       <c r="D12" s="1">
         <v>1</v>
       </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
+      <c r="E12" s="2">
+        <v>1</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1</v>
+      </c>
+      <c r="G12" s="2">
+        <v>1</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
@@ -1638,10 +1710,18 @@
       <c r="D13" s="1">
         <v>1</v>
       </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
+      <c r="E13" s="2">
+        <v>1</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
@@ -1654,10 +1734,18 @@
       <c r="D14" s="1">
         <v>1</v>
       </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
+      <c r="E14" s="2">
+        <v>3</v>
+      </c>
+      <c r="F14" s="2">
+        <v>3</v>
+      </c>
+      <c r="G14" s="2">
+        <v>3</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
@@ -1670,10 +1758,18 @@
       <c r="D15" s="1">
         <v>1</v>
       </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
+      <c r="E15" s="2">
+        <v>1</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
@@ -1686,10 +1782,18 @@
       <c r="D16" s="1">
         <v>1</v>
       </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
+      <c r="E16" s="2">
+        <v>1</v>
+      </c>
+      <c r="F16" s="2">
+        <v>1</v>
+      </c>
+      <c r="G16" s="2">
+        <v>1</v>
+      </c>
+      <c r="H16" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
@@ -1699,15 +1803,23 @@
         <v>23</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D17" s="1">
         <v>1</v>
       </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
+      <c r="E17" s="2">
+        <v>1</v>
+      </c>
+      <c r="F17" s="2">
+        <v>1</v>
+      </c>
+      <c r="G17" s="2">
+        <v>1</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
@@ -1720,10 +1832,18 @@
       <c r="D18" s="1">
         <v>1</v>
       </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
+      <c r="E18" s="2">
+        <v>2</v>
+      </c>
+      <c r="F18" s="2">
+        <v>2</v>
+      </c>
+      <c r="G18" s="2">
+        <v>2</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
@@ -1731,15 +1851,23 @@
         <v>21</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D19" s="1">
         <v>3</v>
       </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
+      <c r="E19" s="2">
+        <v>2</v>
+      </c>
+      <c r="F19" s="2">
+        <v>2</v>
+      </c>
+      <c r="G19" s="2">
+        <v>2</v>
+      </c>
+      <c r="H19" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
@@ -1754,10 +1882,18 @@
       <c r="D20" s="1">
         <v>5</v>
       </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
+      <c r="E20" s="2">
+        <v>3</v>
+      </c>
+      <c r="F20" s="2">
+        <v>3</v>
+      </c>
+      <c r="G20" s="2">
+        <v>0</v>
+      </c>
+      <c r="H20" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
@@ -1829,15 +1965,15 @@
       </c>
       <c r="E27" s="3">
         <f t="shared" ref="E27:H27" si="0">SUM(E3:E26)</f>
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="F27" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="G27" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H27" s="3">
         <f t="shared" si="0"/>

</xml_diff>